<commit_message>
MS-WWSP: Add capture code R327001.
</commit_message>
<xml_diff>
--- a/SharePoint/Docs/MS-WWSP/MS-WWSP_RequirementSpecification.xlsx
+++ b/SharePoint/Docs/MS-WWSP/MS-WWSP_RequirementSpecification.xlsx
@@ -3400,6 +3400,21 @@
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3424,292 +3439,11 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="69">
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -4072,6 +3806,272 @@
         <scheme val="none"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -4199,34 +4199,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I383" tableType="xml" totalsRowShown="0" headerRowDxfId="68" dataDxfId="67">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I383" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
   <autoFilter ref="A19:I383"/>
   <tableColumns count="9">
-    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="66">
+    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="16">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="65">
+    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="15">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Doc_Sect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="64">
+    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="14">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="63">
+    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="13">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Derived" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="62">
+    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="12">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Behavior" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="61">
+    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="11">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Scope" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="60">
+    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="10">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:IsNormative" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="59">
+    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="9">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Verification" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="58">
+    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="8">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:VerificationComment" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -4235,12 +4235,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="57" dataDxfId="55" headerRowBorderDxfId="56" tableBorderDxfId="54" totalsRowBorderDxfId="53">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <autoFilter ref="A12:C15"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Scope" dataDxfId="52"/>
-    <tableColumn id="2" name="Test" dataDxfId="51"/>
-    <tableColumn id="3" name="Description" dataDxfId="50"/>
+    <tableColumn id="1" name="Scope" dataDxfId="2"/>
+    <tableColumn id="2" name="Test" dataDxfId="1"/>
+    <tableColumn id="3" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4536,8 +4536,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:K385"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A105" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A114" sqref="A114:XFD114"/>
+    <sheetView tabSelected="1" topLeftCell="D105" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H114" sqref="H114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -4589,120 +4589,120 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="21">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="48"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="48"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="51" t="s">
+      <c r="B5" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
-      <c r="G5" s="52"/>
-      <c r="H5" s="52"/>
-      <c r="I5" s="52"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="44"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="50"/>
-      <c r="G6" s="50"/>
-      <c r="H6" s="50"/>
-      <c r="I6" s="50"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="42"/>
+      <c r="I6" s="42"/>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="49" t="s">
+      <c r="B7" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="49"/>
-      <c r="D7" s="49"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49"/>
-      <c r="G7" s="49"/>
-      <c r="H7" s="49"/>
-      <c r="I7" s="49"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="41"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="49" t="s">
+      <c r="B8" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="49"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="49"/>
-      <c r="G8" s="49"/>
-      <c r="H8" s="49"/>
-      <c r="I8" s="49"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
     </row>
     <row r="9" spans="1:9" ht="78.75" customHeight="1">
       <c r="A9" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="44" t="s">
+      <c r="B9" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="45"/>
-      <c r="D9" s="45"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="45"/>
-      <c r="G9" s="45"/>
-      <c r="H9" s="45"/>
-      <c r="I9" s="45"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="50"/>
+      <c r="I9" s="50"/>
     </row>
     <row r="10" spans="1:9" ht="33.75" customHeight="1">
       <c r="A10" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="44" t="s">
+      <c r="B10" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="45"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="45"/>
-      <c r="G10" s="45"/>
-      <c r="H10" s="45"/>
-      <c r="I10" s="45"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="50"/>
+      <c r="G10" s="50"/>
+      <c r="H10" s="50"/>
+      <c r="I10" s="50"/>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="45"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="45"/>
+      <c r="I11" s="45"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="24" t="s">
@@ -4714,12 +4714,12 @@
       <c r="C12" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="41"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="41"/>
-      <c r="I12" s="41"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="46"/>
+      <c r="I12" s="46"/>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1">
       <c r="A13" s="25" t="s">
@@ -4731,12 +4731,12 @@
       <c r="C13" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="42"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="42"/>
-      <c r="G13" s="42"/>
-      <c r="H13" s="42"/>
-      <c r="I13" s="42"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="47"/>
+      <c r="F13" s="47"/>
+      <c r="G13" s="47"/>
+      <c r="H13" s="47"/>
+      <c r="I13" s="47"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="25" t="s">
@@ -4748,12 +4748,12 @@
       <c r="C14" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="42"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="42"/>
-      <c r="G14" s="42"/>
-      <c r="H14" s="42"/>
-      <c r="I14" s="42"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="47"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="47"/>
+      <c r="H14" s="47"/>
+      <c r="I14" s="47"/>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="26" t="s">
@@ -4765,57 +4765,57 @@
       <c r="C15" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="43"/>
-      <c r="E15" s="43"/>
-      <c r="F15" s="43"/>
-      <c r="G15" s="43"/>
-      <c r="H15" s="43"/>
-      <c r="I15" s="43"/>
+      <c r="D15" s="48"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="48"/>
+      <c r="H15" s="48"/>
+      <c r="I15" s="48"/>
     </row>
     <row r="16" spans="1:9" ht="30" customHeight="1">
       <c r="A16" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="40" t="s">
+      <c r="B16" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="40"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="40"/>
-      <c r="F16" s="40"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="40"/>
+      <c r="C16" s="45"/>
+      <c r="D16" s="45"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="45"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="45"/>
+      <c r="I16" s="45"/>
     </row>
     <row r="17" spans="1:10" ht="64.5" customHeight="1">
       <c r="A17" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="46" t="s">
+      <c r="B17" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="47"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="47"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
+      <c r="C17" s="52"/>
+      <c r="D17" s="52"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="52"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="52"/>
+      <c r="I17" s="52"/>
     </row>
     <row r="18" spans="1:10" ht="30" customHeight="1">
       <c r="A18" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="40" t="s">
+      <c r="B18" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
-      <c r="F18" s="40"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="45"/>
+      <c r="I18" s="45"/>
     </row>
     <row r="19" spans="1:10" s="32" customFormat="1" ht="30">
       <c r="A19" s="3" t="s">
@@ -7295,7 +7295,7 @@
         <v>15</v>
       </c>
       <c r="H113" s="31" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I113" s="38"/>
       <c r="J113" s="19"/>
@@ -14380,11 +14380,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -14392,191 +14387,196 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A383:I383 A374:K382 A20:J60 I302:I356 A358:J373 I64:I291 J61:J357 A61:H357">
-    <cfRule type="expression" dxfId="49" priority="404">
+    <cfRule type="expression" dxfId="68" priority="404">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="405">
+    <cfRule type="expression" dxfId="67" priority="405">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="47" priority="406">
+    <cfRule type="expression" dxfId="66" priority="406">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F383">
-    <cfRule type="expression" dxfId="46" priority="385">
+    <cfRule type="expression" dxfId="65" priority="385">
       <formula>NOT(VLOOKUP(F383,$A$13:$C$16,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="386">
+    <cfRule type="expression" dxfId="64" priority="386">
       <formula>(VLOOKUP(F383,$A$13:$C$16,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A374:I383 A20:J60 I302:I356 A358:J373 I64:I291 J61:J357 A61:H357">
-    <cfRule type="expression" dxfId="44" priority="393">
+    <cfRule type="expression" dxfId="63" priority="393">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="394">
+    <cfRule type="expression" dxfId="62" priority="394">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="395">
+    <cfRule type="expression" dxfId="61" priority="395">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F374:F382">
-    <cfRule type="expression" dxfId="41" priority="39">
+    <cfRule type="expression" dxfId="60" priority="39">
       <formula>NOT(VLOOKUP(F374,$A$13:$C$16,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="40">
+    <cfRule type="expression" dxfId="59" priority="40">
       <formula>(VLOOKUP(F374,$A$13:$C$16,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I61:I62">
-    <cfRule type="expression" dxfId="39" priority="52">
+    <cfRule type="expression" dxfId="58" priority="52">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="53">
+    <cfRule type="expression" dxfId="57" priority="53">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="54">
+    <cfRule type="expression" dxfId="56" priority="54">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I61:I62">
-    <cfRule type="expression" dxfId="36" priority="47">
+    <cfRule type="expression" dxfId="55" priority="47">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="48">
+    <cfRule type="expression" dxfId="54" priority="48">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="49">
+    <cfRule type="expression" dxfId="53" priority="49">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F292:F301">
-    <cfRule type="expression" dxfId="33" priority="50">
+    <cfRule type="expression" dxfId="52" priority="50">
       <formula>NOT(VLOOKUP(F292,$A$13:$C$16,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="51">
+    <cfRule type="expression" dxfId="51" priority="51">
       <formula>(VLOOKUP(F292,$A$13:$C$16,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I292:I301">
-    <cfRule type="expression" dxfId="31" priority="44">
+    <cfRule type="expression" dxfId="50" priority="44">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="45">
+    <cfRule type="expression" dxfId="49" priority="45">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="46">
+    <cfRule type="expression" dxfId="48" priority="46">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I292:I301">
-    <cfRule type="expression" dxfId="28" priority="41">
+    <cfRule type="expression" dxfId="47" priority="41">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="42">
+    <cfRule type="expression" dxfId="46" priority="42">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="43">
+    <cfRule type="expression" dxfId="45" priority="43">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20:F373">
-    <cfRule type="expression" dxfId="25" priority="34">
+    <cfRule type="expression" dxfId="44" priority="34">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="35">
+    <cfRule type="expression" dxfId="43" priority="35">
       <formula>(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I63">
-    <cfRule type="expression" dxfId="23" priority="22">
+    <cfRule type="expression" dxfId="42" priority="22">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="23">
+    <cfRule type="expression" dxfId="41" priority="23">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="24">
+    <cfRule type="expression" dxfId="40" priority="24">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I63">
-    <cfRule type="expression" dxfId="20" priority="19">
+    <cfRule type="expression" dxfId="39" priority="19">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="20">
+    <cfRule type="expression" dxfId="38" priority="20">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="21">
+    <cfRule type="expression" dxfId="37" priority="21">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I63">
-    <cfRule type="expression" dxfId="17" priority="16">
+    <cfRule type="expression" dxfId="36" priority="16">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="17">
+    <cfRule type="expression" dxfId="35" priority="17">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="18">
+    <cfRule type="expression" dxfId="34" priority="18">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I63">
-    <cfRule type="expression" dxfId="14" priority="13">
+    <cfRule type="expression" dxfId="33" priority="13">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="14">
+    <cfRule type="expression" dxfId="32" priority="14">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="15">
+    <cfRule type="expression" dxfId="31" priority="15">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I357">
-    <cfRule type="expression" dxfId="11" priority="10">
+    <cfRule type="expression" dxfId="30" priority="10">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="11">
+    <cfRule type="expression" dxfId="29" priority="11">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="12">
+    <cfRule type="expression" dxfId="28" priority="12">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I357">
-    <cfRule type="expression" dxfId="8" priority="7">
+    <cfRule type="expression" dxfId="27" priority="7">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="8">
+    <cfRule type="expression" dxfId="26" priority="8">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="9">
+    <cfRule type="expression" dxfId="25" priority="9">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I357">
-    <cfRule type="expression" dxfId="5" priority="4">
+    <cfRule type="expression" dxfId="24" priority="4">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="23" priority="5">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="6">
+    <cfRule type="expression" dxfId="22" priority="6">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I357">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="21" priority="1">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="20" priority="2">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="19" priority="3">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14617,21 +14617,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -14680,10 +14665,32 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -14703,16 +14710,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[MS-WWSP]: Add new cases and capture code for 3 fixed TDIs\TDQs
</commit_message>
<xml_diff>
--- a/SharePoint/Docs/MS-WWSP/MS-WWSP_RequirementSpecification.xlsx
+++ b/SharePoint/Docs/MS-WWSP/MS-WWSP_RequirementSpecification.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16925"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Github\Interop-TestSuites2\SharePoint\Docs\MS-WWSP\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-15" yWindow="60" windowWidth="15405" windowHeight="6900" tabRatio="570"/>
   </bookViews>
@@ -3126,7 +3131,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="0.0.0"/>
@@ -3400,21 +3405,6 @@
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3438,6 +3428,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4289,7 +4294,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4322,9 +4327,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4357,6 +4379,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -4536,21 +4575,19 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:K385"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D105" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H114" sqref="H114"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" style="10" customWidth="1"/>
+    <col min="1" max="1" width="12.375" style="10" customWidth="1"/>
     <col min="2" max="2" width="13" style="3" customWidth="1"/>
     <col min="3" max="3" width="85" style="3" customWidth="1"/>
-    <col min="4" max="4" width="28.5703125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="28.625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12.125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="13.375" style="3" customWidth="1"/>
     <col min="8" max="8" width="23" style="3" customWidth="1"/>
-    <col min="9" max="9" width="28.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="28.75" style="3" customWidth="1"/>
     <col min="10" max="10" width="9" style="3" customWidth="1"/>
     <col min="11" max="16384" width="9" style="3"/>
   </cols>
@@ -4589,120 +4626,120 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="21">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
+      <c r="B4" s="48"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="43" t="s">
+      <c r="B5" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="44"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="52"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="42"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="50"/>
+      <c r="I6" s="50"/>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="41" t="s">
+      <c r="B7" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="41"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="41"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="49"/>
+      <c r="H7" s="49"/>
+      <c r="I7" s="49"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="41" t="s">
+      <c r="B8" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="41"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="49"/>
+      <c r="G8" s="49"/>
+      <c r="H8" s="49"/>
+      <c r="I8" s="49"/>
     </row>
     <row r="9" spans="1:9" ht="78.75" customHeight="1">
       <c r="A9" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="49" t="s">
+      <c r="B9" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="50"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
-      <c r="F9" s="50"/>
-      <c r="G9" s="50"/>
-      <c r="H9" s="50"/>
-      <c r="I9" s="50"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="45"/>
+      <c r="I9" s="45"/>
     </row>
     <row r="10" spans="1:9" ht="33.75" customHeight="1">
       <c r="A10" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="49" t="s">
+      <c r="B10" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="50"/>
-      <c r="D10" s="50"/>
-      <c r="E10" s="50"/>
-      <c r="F10" s="50"/>
-      <c r="G10" s="50"/>
-      <c r="H10" s="50"/>
-      <c r="I10" s="50"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="45"/>
+      <c r="I10" s="45"/>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="45" t="s">
+      <c r="B11" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="45"/>
-      <c r="D11" s="45"/>
-      <c r="E11" s="45"/>
-      <c r="F11" s="45"/>
-      <c r="G11" s="45"/>
-      <c r="H11" s="45"/>
-      <c r="I11" s="45"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="40"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="24" t="s">
@@ -4714,12 +4751,12 @@
       <c r="C12" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="46"/>
-      <c r="E12" s="46"/>
-      <c r="F12" s="46"/>
-      <c r="G12" s="46"/>
-      <c r="H12" s="46"/>
-      <c r="I12" s="46"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="41"/>
+      <c r="I12" s="41"/>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1">
       <c r="A13" s="25" t="s">
@@ -4731,12 +4768,12 @@
       <c r="C13" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="47"/>
-      <c r="E13" s="47"/>
-      <c r="F13" s="47"/>
-      <c r="G13" s="47"/>
-      <c r="H13" s="47"/>
-      <c r="I13" s="47"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="42"/>
+      <c r="I13" s="42"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="25" t="s">
@@ -4748,12 +4785,12 @@
       <c r="C14" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="47"/>
-      <c r="E14" s="47"/>
-      <c r="F14" s="47"/>
-      <c r="G14" s="47"/>
-      <c r="H14" s="47"/>
-      <c r="I14" s="47"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="42"/>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="26" t="s">
@@ -4765,57 +4802,57 @@
       <c r="C15" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="48"/>
-      <c r="E15" s="48"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="48"/>
-      <c r="H15" s="48"/>
-      <c r="I15" s="48"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="43"/>
+      <c r="I15" s="43"/>
     </row>
     <row r="16" spans="1:9" ht="30" customHeight="1">
       <c r="A16" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="45" t="s">
+      <c r="B16" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="45"/>
-      <c r="D16" s="45"/>
-      <c r="E16" s="45"/>
-      <c r="F16" s="45"/>
-      <c r="G16" s="45"/>
-      <c r="H16" s="45"/>
-      <c r="I16" s="45"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="40"/>
     </row>
     <row r="17" spans="1:10" ht="64.5" customHeight="1">
       <c r="A17" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="51" t="s">
+      <c r="B17" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="52"/>
-      <c r="D17" s="52"/>
-      <c r="E17" s="52"/>
-      <c r="F17" s="52"/>
-      <c r="G17" s="52"/>
-      <c r="H17" s="52"/>
-      <c r="I17" s="52"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
     </row>
     <row r="18" spans="1:10" ht="30" customHeight="1">
       <c r="A18" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="45" t="s">
+      <c r="B18" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="45"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="45"/>
-      <c r="F18" s="45"/>
-      <c r="G18" s="45"/>
-      <c r="H18" s="45"/>
-      <c r="I18" s="45"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
     </row>
     <row r="19" spans="1:10" s="32" customFormat="1" ht="30">
       <c r="A19" s="3" t="s">
@@ -4978,7 +5015,7 @@
       <c r="I24" s="22"/>
       <c r="J24" s="22"/>
     </row>
-    <row r="25" spans="1:10" s="33" customFormat="1" ht="30">
+    <row r="25" spans="1:10" s="33" customFormat="1">
       <c r="A25" s="21" t="s">
         <v>54</v>
       </c>
@@ -5082,7 +5119,7 @@
       <c r="I28" s="22"/>
       <c r="J28" s="22"/>
     </row>
-    <row r="29" spans="1:10" s="33" customFormat="1" ht="30">
+    <row r="29" spans="1:10" s="33" customFormat="1">
       <c r="A29" s="21" t="s">
         <v>63</v>
       </c>
@@ -5186,7 +5223,7 @@
       <c r="I32" s="22"/>
       <c r="J32" s="22"/>
     </row>
-    <row r="33" spans="1:10" ht="30">
+    <row r="33" spans="1:10">
       <c r="A33" s="21" t="s">
         <v>71</v>
       </c>
@@ -5264,7 +5301,7 @@
       <c r="I35" s="19"/>
       <c r="J35" s="19"/>
     </row>
-    <row r="36" spans="1:10" ht="30">
+    <row r="36" spans="1:10">
       <c r="A36" s="21" t="s">
         <v>77</v>
       </c>
@@ -5706,7 +5743,7 @@
       <c r="I52" s="19"/>
       <c r="J52" s="19"/>
     </row>
-    <row r="53" spans="1:10" ht="45">
+    <row r="53" spans="1:10" ht="30">
       <c r="A53" s="21" t="s">
         <v>113</v>
       </c>
@@ -5758,7 +5795,7 @@
       <c r="I54" s="19"/>
       <c r="J54" s="19"/>
     </row>
-    <row r="55" spans="1:10" ht="30">
+    <row r="55" spans="1:10">
       <c r="A55" s="21" t="s">
         <v>117</v>
       </c>
@@ -5888,7 +5925,7 @@
       <c r="I59" s="19"/>
       <c r="J59" s="19"/>
     </row>
-    <row r="60" spans="1:10" ht="45">
+    <row r="60" spans="1:10" ht="30">
       <c r="A60" s="21" t="s">
         <v>127</v>
       </c>
@@ -5942,7 +5979,7 @@
       <c r="I61" s="19"/>
       <c r="J61" s="19"/>
     </row>
-    <row r="62" spans="1:10" ht="45">
+    <row r="62" spans="1:10" ht="30">
       <c r="A62" s="21" t="s">
         <v>131</v>
       </c>
@@ -5968,7 +6005,7 @@
       <c r="I62" s="19"/>
       <c r="J62" s="19"/>
     </row>
-    <row r="63" spans="1:10" ht="45">
+    <row r="63" spans="1:10" ht="30">
       <c r="A63" s="21" t="s">
         <v>133</v>
       </c>
@@ -5994,7 +6031,7 @@
       <c r="I63" s="19"/>
       <c r="J63" s="19"/>
     </row>
-    <row r="64" spans="1:10" ht="60">
+    <row r="64" spans="1:10" ht="45">
       <c r="A64" s="21" t="s">
         <v>135</v>
       </c>
@@ -6022,7 +6059,7 @@
       </c>
       <c r="J64" s="19"/>
     </row>
-    <row r="65" spans="1:10" ht="60">
+    <row r="65" spans="1:10" ht="45">
       <c r="A65" s="21" t="s">
         <v>136</v>
       </c>
@@ -6074,7 +6111,7 @@
       <c r="I66" s="19"/>
       <c r="J66" s="19"/>
     </row>
-    <row r="67" spans="1:10" ht="30">
+    <row r="67" spans="1:10">
       <c r="A67" s="21" t="s">
         <v>140</v>
       </c>
@@ -6178,7 +6215,7 @@
       <c r="I70" s="19"/>
       <c r="J70" s="19"/>
     </row>
-    <row r="71" spans="1:10" ht="30">
+    <row r="71" spans="1:10">
       <c r="A71" s="21" t="s">
         <v>149</v>
       </c>
@@ -6334,7 +6371,7 @@
       <c r="I76" s="19"/>
       <c r="J76" s="19"/>
     </row>
-    <row r="77" spans="1:10" ht="45">
+    <row r="77" spans="1:10" ht="30">
       <c r="A77" s="21" t="s">
         <v>161</v>
       </c>
@@ -6412,7 +6449,7 @@
       <c r="I79" s="19"/>
       <c r="J79" s="19"/>
     </row>
-    <row r="80" spans="1:10" ht="45">
+    <row r="80" spans="1:10" ht="30">
       <c r="A80" s="21" t="s">
         <v>168</v>
       </c>
@@ -6464,7 +6501,7 @@
       <c r="I81" s="19"/>
       <c r="J81" s="19"/>
     </row>
-    <row r="82" spans="1:10" ht="30">
+    <row r="82" spans="1:10">
       <c r="A82" s="21" t="s">
         <v>173</v>
       </c>
@@ -6516,7 +6553,7 @@
       <c r="I83" s="19"/>
       <c r="J83" s="19"/>
     </row>
-    <row r="84" spans="1:10" ht="45">
+    <row r="84" spans="1:10" ht="30">
       <c r="A84" s="21" t="s">
         <v>175</v>
       </c>
@@ -6568,7 +6605,7 @@
       <c r="I85" s="19"/>
       <c r="J85" s="19"/>
     </row>
-    <row r="86" spans="1:10" ht="45">
+    <row r="86" spans="1:10" ht="30">
       <c r="A86" s="21" t="s">
         <v>179</v>
       </c>
@@ -6802,7 +6839,7 @@
       <c r="I94" s="19"/>
       <c r="J94" s="19"/>
     </row>
-    <row r="95" spans="1:10" ht="30">
+    <row r="95" spans="1:10">
       <c r="A95" s="21" t="s">
         <v>198</v>
       </c>
@@ -6958,7 +6995,7 @@
       <c r="I100" s="19"/>
       <c r="J100" s="19"/>
     </row>
-    <row r="101" spans="1:10" ht="30">
+    <row r="101" spans="1:10">
       <c r="A101" s="21" t="s">
         <v>213</v>
       </c>
@@ -7326,7 +7363,7 @@
       <c r="I114" s="19"/>
       <c r="J114" s="19"/>
     </row>
-    <row r="115" spans="1:10" ht="210">
+    <row r="115" spans="1:10" ht="195">
       <c r="A115" s="21" t="s">
         <v>240</v>
       </c>
@@ -7482,7 +7519,7 @@
       <c r="I120" s="19"/>
       <c r="J120" s="19"/>
     </row>
-    <row r="121" spans="1:10" ht="30">
+    <row r="121" spans="1:10">
       <c r="A121" s="21" t="s">
         <v>251</v>
       </c>
@@ -7508,7 +7545,7 @@
       <c r="I121" s="19"/>
       <c r="J121" s="19"/>
     </row>
-    <row r="122" spans="1:10" ht="75">
+    <row r="122" spans="1:10" ht="60">
       <c r="A122" s="21" t="s">
         <v>252</v>
       </c>
@@ -7534,7 +7571,7 @@
       <c r="I122" s="19"/>
       <c r="J122" s="19"/>
     </row>
-    <row r="123" spans="1:10" ht="45">
+    <row r="123" spans="1:10" ht="30">
       <c r="A123" s="21" t="s">
         <v>254</v>
       </c>
@@ -7586,7 +7623,7 @@
       <c r="I124" s="19"/>
       <c r="J124" s="19"/>
     </row>
-    <row r="125" spans="1:10" ht="30">
+    <row r="125" spans="1:10">
       <c r="A125" s="21" t="s">
         <v>258</v>
       </c>
@@ -7716,7 +7753,7 @@
       <c r="I129" s="19"/>
       <c r="J129" s="19"/>
     </row>
-    <row r="130" spans="1:10" ht="30">
+    <row r="130" spans="1:10">
       <c r="A130" s="21" t="s">
         <v>267</v>
       </c>
@@ -7742,7 +7779,7 @@
       <c r="I130" s="19"/>
       <c r="J130" s="19"/>
     </row>
-    <row r="131" spans="1:10" ht="30">
+    <row r="131" spans="1:10">
       <c r="A131" s="21" t="s">
         <v>270</v>
       </c>
@@ -7794,7 +7831,7 @@
       <c r="I132" s="19"/>
       <c r="J132" s="19"/>
     </row>
-    <row r="133" spans="1:10" ht="30">
+    <row r="133" spans="1:10">
       <c r="A133" s="21" t="s">
         <v>274</v>
       </c>
@@ -7846,7 +7883,7 @@
       <c r="I134" s="19"/>
       <c r="J134" s="19"/>
     </row>
-    <row r="135" spans="1:10" ht="45">
+    <row r="135" spans="1:10" ht="30">
       <c r="A135" s="21" t="s">
         <v>276</v>
       </c>
@@ -7872,7 +7909,7 @@
       <c r="I135" s="19"/>
       <c r="J135" s="19"/>
     </row>
-    <row r="136" spans="1:10" ht="165">
+    <row r="136" spans="1:10" ht="150">
       <c r="A136" s="21" t="s">
         <v>279</v>
       </c>
@@ -7924,7 +7961,7 @@
       <c r="I137" s="19"/>
       <c r="J137" s="19"/>
     </row>
-    <row r="138" spans="1:10" ht="45">
+    <row r="138" spans="1:10" ht="30">
       <c r="A138" s="21" t="s">
         <v>282</v>
       </c>
@@ -8058,7 +8095,7 @@
       <c r="I142" s="19"/>
       <c r="J142" s="19"/>
     </row>
-    <row r="143" spans="1:10" ht="30">
+    <row r="143" spans="1:10">
       <c r="A143" s="21" t="s">
         <v>293</v>
       </c>
@@ -8240,7 +8277,7 @@
       <c r="I149" s="19"/>
       <c r="J149" s="19"/>
     </row>
-    <row r="150" spans="1:10" ht="45">
+    <row r="150" spans="1:10" ht="30">
       <c r="A150" s="21" t="s">
         <v>307</v>
       </c>
@@ -8396,7 +8433,7 @@
       <c r="I155" s="19"/>
       <c r="J155" s="19"/>
     </row>
-    <row r="156" spans="1:10" ht="45">
+    <row r="156" spans="1:10" ht="30">
       <c r="A156" s="21" t="s">
         <v>319</v>
       </c>
@@ -8500,7 +8537,7 @@
       <c r="I159" s="19"/>
       <c r="J159" s="19"/>
     </row>
-    <row r="160" spans="1:10" ht="30">
+    <row r="160" spans="1:10">
       <c r="A160" s="21" t="s">
         <v>327</v>
       </c>
@@ -8526,7 +8563,7 @@
       <c r="I160" s="19"/>
       <c r="J160" s="19"/>
     </row>
-    <row r="161" spans="1:10" ht="45">
+    <row r="161" spans="1:10" ht="30">
       <c r="A161" s="21" t="s">
         <v>330</v>
       </c>
@@ -8604,7 +8641,7 @@
       <c r="I163" s="19"/>
       <c r="J163" s="19"/>
     </row>
-    <row r="164" spans="1:10" ht="30">
+    <row r="164" spans="1:10">
       <c r="A164" s="21" t="s">
         <v>337</v>
       </c>
@@ -8682,7 +8719,7 @@
       <c r="I166" s="19"/>
       <c r="J166" s="19"/>
     </row>
-    <row r="167" spans="1:10" ht="45">
+    <row r="167" spans="1:10" ht="30">
       <c r="A167" s="21" t="s">
         <v>343</v>
       </c>
@@ -8838,7 +8875,7 @@
       <c r="I172" s="19"/>
       <c r="J172" s="19"/>
     </row>
-    <row r="173" spans="1:10" ht="30">
+    <row r="173" spans="1:10">
       <c r="A173" s="21" t="s">
         <v>356</v>
       </c>
@@ -8864,7 +8901,7 @@
       <c r="I173" s="19"/>
       <c r="J173" s="19"/>
     </row>
-    <row r="174" spans="1:10" ht="225">
+    <row r="174" spans="1:10" ht="210">
       <c r="A174" s="21" t="s">
         <v>359</v>
       </c>
@@ -8942,7 +8979,7 @@
       <c r="I176" s="19"/>
       <c r="J176" s="19"/>
     </row>
-    <row r="177" spans="1:10" ht="75">
+    <row r="177" spans="1:10" ht="60">
       <c r="A177" s="21" t="s">
         <v>365</v>
       </c>
@@ -9150,7 +9187,7 @@
       <c r="I184" s="19"/>
       <c r="J184" s="19"/>
     </row>
-    <row r="185" spans="1:10" ht="30">
+    <row r="185" spans="1:10">
       <c r="A185" s="21" t="s">
         <v>382</v>
       </c>
@@ -9176,7 +9213,7 @@
       <c r="I185" s="19"/>
       <c r="J185" s="19"/>
     </row>
-    <row r="186" spans="1:10" ht="30">
+    <row r="186" spans="1:10">
       <c r="A186" s="21" t="s">
         <v>385</v>
       </c>
@@ -9280,7 +9317,7 @@
       <c r="I189" s="19"/>
       <c r="J189" s="19"/>
     </row>
-    <row r="190" spans="1:10" ht="30">
+    <row r="190" spans="1:10">
       <c r="A190" s="21" t="s">
         <v>393</v>
       </c>
@@ -9306,7 +9343,7 @@
       <c r="I190" s="19"/>
       <c r="J190" s="19"/>
     </row>
-    <row r="191" spans="1:10" ht="120">
+    <row r="191" spans="1:10" ht="105">
       <c r="A191" s="21" t="s">
         <v>396</v>
       </c>
@@ -9462,7 +9499,7 @@
       <c r="I196" s="19"/>
       <c r="J196" s="19"/>
     </row>
-    <row r="197" spans="1:10" ht="45">
+    <row r="197" spans="1:10" ht="30">
       <c r="A197" s="21" t="s">
         <v>409</v>
       </c>
@@ -9514,7 +9551,7 @@
       <c r="I198" s="19"/>
       <c r="J198" s="19"/>
     </row>
-    <row r="199" spans="1:10" ht="45">
+    <row r="199" spans="1:10" ht="30">
       <c r="A199" s="21" t="s">
         <v>413</v>
       </c>
@@ -9618,7 +9655,7 @@
       <c r="I202" s="19"/>
       <c r="J202" s="19"/>
     </row>
-    <row r="203" spans="1:10" ht="30">
+    <row r="203" spans="1:10">
       <c r="A203" s="21" t="s">
         <v>421</v>
       </c>
@@ -9644,7 +9681,7 @@
       <c r="I203" s="19"/>
       <c r="J203" s="19"/>
     </row>
-    <row r="204" spans="1:10" ht="45">
+    <row r="204" spans="1:10" ht="30">
       <c r="A204" s="21" t="s">
         <v>424</v>
       </c>
@@ -9670,7 +9707,7 @@
       <c r="I204" s="19"/>
       <c r="J204" s="19"/>
     </row>
-    <row r="205" spans="1:10" ht="30">
+    <row r="205" spans="1:10">
       <c r="A205" s="21" t="s">
         <v>426</v>
       </c>
@@ -9956,7 +9993,7 @@
       <c r="I215" s="19"/>
       <c r="J215" s="19"/>
     </row>
-    <row r="216" spans="1:10" ht="45">
+    <row r="216" spans="1:10" ht="30">
       <c r="A216" s="21" t="s">
         <v>450</v>
       </c>
@@ -9982,7 +10019,7 @@
       <c r="I216" s="19"/>
       <c r="J216" s="19"/>
     </row>
-    <row r="217" spans="1:10" ht="45">
+    <row r="217" spans="1:10" ht="30">
       <c r="A217" s="21" t="s">
         <v>452</v>
       </c>
@@ -10112,7 +10149,7 @@
       <c r="I221" s="19"/>
       <c r="J221" s="19"/>
     </row>
-    <row r="222" spans="1:10" ht="60">
+    <row r="222" spans="1:10" ht="45">
       <c r="A222" s="21" t="s">
         <v>462</v>
       </c>
@@ -10164,7 +10201,7 @@
       <c r="I223" s="19"/>
       <c r="J223" s="19"/>
     </row>
-    <row r="224" spans="1:10" ht="45">
+    <row r="224" spans="1:10" ht="30">
       <c r="A224" s="21" t="s">
         <v>466</v>
       </c>
@@ -10190,7 +10227,7 @@
       <c r="I224" s="19"/>
       <c r="J224" s="19"/>
     </row>
-    <row r="225" spans="1:10" ht="45">
+    <row r="225" spans="1:10" ht="30">
       <c r="A225" s="21" t="s">
         <v>468</v>
       </c>
@@ -10216,7 +10253,7 @@
       <c r="I225" s="19"/>
       <c r="J225" s="19"/>
     </row>
-    <row r="226" spans="1:10" ht="45">
+    <row r="226" spans="1:10" ht="30">
       <c r="A226" s="21" t="s">
         <v>470</v>
       </c>
@@ -10242,7 +10279,7 @@
       <c r="I226" s="19"/>
       <c r="J226" s="19"/>
     </row>
-    <row r="227" spans="1:10" ht="45">
+    <row r="227" spans="1:10" ht="30">
       <c r="A227" s="21" t="s">
         <v>472</v>
       </c>
@@ -10294,7 +10331,7 @@
       <c r="I228" s="19"/>
       <c r="J228" s="19"/>
     </row>
-    <row r="229" spans="1:10" ht="45">
+    <row r="229" spans="1:10" ht="30">
       <c r="A229" s="21" t="s">
         <v>476</v>
       </c>
@@ -10346,7 +10383,7 @@
       <c r="I230" s="19"/>
       <c r="J230" s="19"/>
     </row>
-    <row r="231" spans="1:10" ht="45">
+    <row r="231" spans="1:10" ht="30">
       <c r="A231" s="21" t="s">
         <v>480</v>
       </c>
@@ -10554,7 +10591,7 @@
       <c r="I238" s="19"/>
       <c r="J238" s="19"/>
     </row>
-    <row r="239" spans="1:10" ht="45">
+    <row r="239" spans="1:10" ht="30">
       <c r="A239" s="21" t="s">
         <v>496</v>
       </c>
@@ -10658,7 +10695,7 @@
       <c r="I242" s="19"/>
       <c r="J242" s="19"/>
     </row>
-    <row r="243" spans="1:10" ht="45">
+    <row r="243" spans="1:10" ht="30">
       <c r="A243" s="21" t="s">
         <v>504</v>
       </c>
@@ -10762,7 +10799,7 @@
       <c r="I246" s="19"/>
       <c r="J246" s="19"/>
     </row>
-    <row r="247" spans="1:10" ht="45">
+    <row r="247" spans="1:10" ht="30">
       <c r="A247" s="21" t="s">
         <v>512</v>
       </c>
@@ -10814,7 +10851,7 @@
       <c r="I248" s="19"/>
       <c r="J248" s="19"/>
     </row>
-    <row r="249" spans="1:10" ht="45">
+    <row r="249" spans="1:10" ht="30">
       <c r="A249" s="21" t="s">
         <v>516</v>
       </c>
@@ -10866,7 +10903,7 @@
       <c r="I250" s="19"/>
       <c r="J250" s="19"/>
     </row>
-    <row r="251" spans="1:10" ht="45">
+    <row r="251" spans="1:10" ht="30">
       <c r="A251" s="21" t="s">
         <v>520</v>
       </c>
@@ -10918,7 +10955,7 @@
       <c r="I252" s="19"/>
       <c r="J252" s="19"/>
     </row>
-    <row r="253" spans="1:10" ht="45">
+    <row r="253" spans="1:10" ht="30">
       <c r="A253" s="21" t="s">
         <v>524</v>
       </c>
@@ -10970,7 +11007,7 @@
       <c r="I254" s="19"/>
       <c r="J254" s="19"/>
     </row>
-    <row r="255" spans="1:10" ht="45">
+    <row r="255" spans="1:10" ht="30">
       <c r="A255" s="21" t="s">
         <v>528</v>
       </c>
@@ -11022,7 +11059,7 @@
       <c r="I256" s="19"/>
       <c r="J256" s="19"/>
     </row>
-    <row r="257" spans="1:10" ht="45">
+    <row r="257" spans="1:10" ht="30">
       <c r="A257" s="21" t="s">
         <v>532</v>
       </c>
@@ -11074,7 +11111,7 @@
       <c r="I258" s="19"/>
       <c r="J258" s="19"/>
     </row>
-    <row r="259" spans="1:10" ht="45">
+    <row r="259" spans="1:10" ht="30">
       <c r="A259" s="21" t="s">
         <v>536</v>
       </c>
@@ -11126,7 +11163,7 @@
       <c r="I260" s="19"/>
       <c r="J260" s="19"/>
     </row>
-    <row r="261" spans="1:10" ht="45">
+    <row r="261" spans="1:10" ht="30">
       <c r="A261" s="21" t="s">
         <v>540</v>
       </c>
@@ -11178,7 +11215,7 @@
       <c r="I262" s="19"/>
       <c r="J262" s="19"/>
     </row>
-    <row r="263" spans="1:10" ht="45">
+    <row r="263" spans="1:10" ht="30">
       <c r="A263" s="21" t="s">
         <v>544</v>
       </c>
@@ -11858,7 +11895,7 @@
       <c r="I288" s="19"/>
       <c r="J288" s="19"/>
     </row>
-    <row r="289" spans="1:10" ht="60">
+    <row r="289" spans="1:10" ht="45">
       <c r="A289" s="21" t="s">
         <v>590</v>
       </c>
@@ -12066,7 +12103,7 @@
       <c r="I296" s="22"/>
       <c r="J296" s="19"/>
     </row>
-    <row r="297" spans="1:10" s="33" customFormat="1" ht="45">
+    <row r="297" spans="1:10" s="33" customFormat="1" ht="30">
       <c r="A297" s="21" t="s">
         <v>738</v>
       </c>
@@ -12248,7 +12285,7 @@
       <c r="I303" s="19"/>
       <c r="J303" s="19"/>
     </row>
-    <row r="304" spans="1:10" ht="45">
+    <row r="304" spans="1:10" ht="30">
       <c r="A304" s="21" t="s">
         <v>601</v>
       </c>
@@ -12352,7 +12389,7 @@
       <c r="I307" s="19"/>
       <c r="J307" s="19"/>
     </row>
-    <row r="308" spans="1:10" ht="30">
+    <row r="308" spans="1:10">
       <c r="A308" s="21" t="s">
         <v>609</v>
       </c>
@@ -12378,7 +12415,7 @@
       <c r="I308" s="19"/>
       <c r="J308" s="19"/>
     </row>
-    <row r="309" spans="1:10" ht="45">
+    <row r="309" spans="1:10" ht="30">
       <c r="A309" s="21" t="s">
         <v>612</v>
       </c>
@@ -12456,7 +12493,7 @@
       <c r="I311" s="19"/>
       <c r="J311" s="19"/>
     </row>
-    <row r="312" spans="1:10" ht="30">
+    <row r="312" spans="1:10">
       <c r="A312" s="21" t="s">
         <v>619</v>
       </c>
@@ -12508,7 +12545,7 @@
       <c r="I313" s="19"/>
       <c r="J313" s="19"/>
     </row>
-    <row r="314" spans="1:10" ht="30">
+    <row r="314" spans="1:10">
       <c r="A314" s="21" t="s">
         <v>623</v>
       </c>
@@ -12709,13 +12746,13 @@
         <v>19</v>
       </c>
       <c r="F321" s="21" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G321" s="21" t="s">
         <v>15</v>
       </c>
       <c r="H321" s="21" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I321" s="19"/>
       <c r="J321" s="19"/>
@@ -12824,7 +12861,7 @@
       <c r="I325" s="19"/>
       <c r="J325" s="19"/>
     </row>
-    <row r="326" spans="1:10" ht="60">
+    <row r="326" spans="1:10" ht="45">
       <c r="A326" s="21" t="s">
         <v>648</v>
       </c>
@@ -12928,7 +12965,7 @@
       <c r="I329" s="19"/>
       <c r="J329" s="19"/>
     </row>
-    <row r="330" spans="1:10" ht="75">
+    <row r="330" spans="1:10" ht="60">
       <c r="A330" s="21" t="s">
         <v>657</v>
       </c>
@@ -13162,7 +13199,7 @@
       <c r="I338" s="19"/>
       <c r="J338" s="19"/>
     </row>
-    <row r="339" spans="1:10" ht="30">
+    <row r="339" spans="1:10">
       <c r="A339" s="21" t="s">
         <v>674</v>
       </c>
@@ -13266,7 +13303,7 @@
       <c r="I342" s="19"/>
       <c r="J342" s="19"/>
     </row>
-    <row r="343" spans="1:10" ht="30">
+    <row r="343" spans="1:10">
       <c r="A343" s="21" t="s">
         <v>682</v>
       </c>
@@ -13318,7 +13355,7 @@
       <c r="I344" s="19"/>
       <c r="J344" s="19"/>
     </row>
-    <row r="345" spans="1:10" ht="240">
+    <row r="345" spans="1:10" ht="225">
       <c r="A345" s="21" t="s">
         <v>686</v>
       </c>
@@ -13783,13 +13820,13 @@
         <v>22</v>
       </c>
       <c r="F362" s="21" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G362" s="21" t="s">
         <v>15</v>
       </c>
       <c r="H362" s="21" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I362" s="19"/>
       <c r="J362" s="19"/>
@@ -13809,13 +13846,13 @@
         <v>22</v>
       </c>
       <c r="F363" s="21" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G363" s="21" t="s">
         <v>15</v>
       </c>
       <c r="H363" s="21" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I363" s="19"/>
       <c r="J363" s="19"/>
@@ -13835,18 +13872,18 @@
         <v>22</v>
       </c>
       <c r="F364" s="21" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G364" s="21" t="s">
         <v>15</v>
       </c>
       <c r="H364" s="21" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I364" s="19"/>
       <c r="J364" s="19"/>
     </row>
-    <row r="365" spans="1:10" ht="60">
+    <row r="365" spans="1:10" ht="45">
       <c r="A365" s="21" t="s">
         <v>716</v>
       </c>
@@ -13861,13 +13898,13 @@
         <v>22</v>
       </c>
       <c r="F365" s="21" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G365" s="21" t="s">
         <v>15</v>
       </c>
       <c r="H365" s="21" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I365" s="19"/>
       <c r="J365" s="19"/>
@@ -13887,18 +13924,18 @@
         <v>22</v>
       </c>
       <c r="F366" s="21" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G366" s="21" t="s">
         <v>15</v>
       </c>
       <c r="H366" s="21" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I366" s="19"/>
       <c r="J366" s="19"/>
     </row>
-    <row r="367" spans="1:10" ht="60">
+    <row r="367" spans="1:10" ht="45">
       <c r="A367" s="21" t="s">
         <v>719</v>
       </c>
@@ -13913,13 +13950,13 @@
         <v>22</v>
       </c>
       <c r="F367" s="21" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G367" s="21" t="s">
         <v>15</v>
       </c>
       <c r="H367" s="21" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I367" s="19"/>
       <c r="J367" s="19"/>
@@ -14042,7 +14079,7 @@
       </c>
       <c r="J371" s="19"/>
     </row>
-    <row r="372" spans="1:11" ht="60">
+    <row r="372" spans="1:11" ht="45">
       <c r="A372" s="21" t="s">
         <v>725</v>
       </c>
@@ -14156,7 +14193,7 @@
       <c r="J375" s="37"/>
       <c r="K375" s="37"/>
     </row>
-    <row r="376" spans="1:11" customFormat="1" ht="30">
+    <row r="376" spans="1:11" customFormat="1">
       <c r="A376" s="27" t="s">
         <v>749</v>
       </c>
@@ -14210,7 +14247,7 @@
       <c r="J377" s="37"/>
       <c r="K377" s="37"/>
     </row>
-    <row r="378" spans="1:11" customFormat="1" ht="30">
+    <row r="378" spans="1:11" customFormat="1">
       <c r="A378" s="27" t="s">
         <v>751</v>
       </c>
@@ -14291,7 +14328,7 @@
       <c r="J380" s="37"/>
       <c r="K380" s="37"/>
     </row>
-    <row r="381" spans="1:11" customFormat="1" ht="30">
+    <row r="381" spans="1:11" customFormat="1">
       <c r="A381" s="27" t="s">
         <v>754</v>
       </c>
@@ -14318,7 +14355,7 @@
       <c r="J381" s="37"/>
       <c r="K381" s="37"/>
     </row>
-    <row r="382" spans="1:11" customFormat="1" ht="30">
+    <row r="382" spans="1:11" customFormat="1">
       <c r="A382" s="27" t="s">
         <v>791</v>
       </c>
@@ -14345,7 +14382,7 @@
       <c r="J382" s="37"/>
       <c r="K382" s="37"/>
     </row>
-    <row r="383" spans="1:11" s="31" customFormat="1" ht="45">
+    <row r="383" spans="1:11" s="31" customFormat="1" ht="30">
       <c r="A383" s="27" t="s">
         <v>755</v>
       </c>
@@ -14380,6 +14417,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -14387,14 +14429,9 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A383:I383 A374:K382 A20:J60 I302:I356 A358:J373 I64:I291 J61:J357 A61:H357">
+  <conditionalFormatting sqref="A383:I383 A374:K382 A20:J60 I302:I356 I64:I291 J61:J357 A61:H357 A358:J373">
     <cfRule type="expression" dxfId="68" priority="404">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
@@ -14413,7 +14450,7 @@
       <formula>(VLOOKUP(F383,$A$13:$C$16,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A374:I383 A20:J60 I302:I356 A358:J373 I64:I291 J61:J357 A61:H357">
+  <conditionalFormatting sqref="A374:I383 A20:J60 I302:I356 I64:I291 J61:J357 A61:H357 A358:J373">
     <cfRule type="expression" dxfId="63" priority="393">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
@@ -14581,7 +14618,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 F302:F373 F20:F291">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 F20:F291 F302:F373">
       <formula1>$A$13:$A$15</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4 E20:E383">
@@ -14607,7 +14644,7 @@
     <oddFooter>&amp;F&amp;RPage &amp;P</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="C3 B19:B111 B114:B281 B283:B331 B353:B360 B333:B351 B361:B385" numberStoredAsText="1"/>
+    <ignoredError sqref="C3 B19:B332 B352:B360 B333:B351 B361:B385" numberStoredAsText="1"/>
   </ignoredErrors>
   <tableParts count="2">
     <tablePart r:id="rId2"/>
@@ -14617,6 +14654,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -14665,12 +14708,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -14681,6 +14718,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14695,20 +14746,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
[MS-WWSP]: Fix watchman warnings
</commit_message>
<xml_diff>
--- a/SharePoint/Docs/MS-WWSP/MS-WWSP_RequirementSpecification.xlsx
+++ b/SharePoint/Docs/MS-WWSP/MS-WWSP_RequirementSpecification.xlsx
@@ -3405,6 +3405,21 @@
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3428,21 +3443,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4626,120 +4626,120 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="21">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="48"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="48"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="51" t="s">
+      <c r="B5" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
-      <c r="G5" s="52"/>
-      <c r="H5" s="52"/>
-      <c r="I5" s="52"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="44"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="50"/>
-      <c r="G6" s="50"/>
-      <c r="H6" s="50"/>
-      <c r="I6" s="50"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="42"/>
+      <c r="I6" s="42"/>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="49" t="s">
+      <c r="B7" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="49"/>
-      <c r="D7" s="49"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49"/>
-      <c r="G7" s="49"/>
-      <c r="H7" s="49"/>
-      <c r="I7" s="49"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="41"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="49" t="s">
+      <c r="B8" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="49"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="49"/>
-      <c r="G8" s="49"/>
-      <c r="H8" s="49"/>
-      <c r="I8" s="49"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
     </row>
     <row r="9" spans="1:9" ht="78.75" customHeight="1">
       <c r="A9" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="44" t="s">
+      <c r="B9" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="45"/>
-      <c r="D9" s="45"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="45"/>
-      <c r="G9" s="45"/>
-      <c r="H9" s="45"/>
-      <c r="I9" s="45"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="50"/>
+      <c r="I9" s="50"/>
     </row>
     <row r="10" spans="1:9" ht="33.75" customHeight="1">
       <c r="A10" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="44" t="s">
+      <c r="B10" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="45"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="45"/>
-      <c r="G10" s="45"/>
-      <c r="H10" s="45"/>
-      <c r="I10" s="45"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="50"/>
+      <c r="G10" s="50"/>
+      <c r="H10" s="50"/>
+      <c r="I10" s="50"/>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="45"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="45"/>
+      <c r="I11" s="45"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="24" t="s">
@@ -4751,12 +4751,12 @@
       <c r="C12" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="41"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="41"/>
-      <c r="I12" s="41"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="46"/>
+      <c r="I12" s="46"/>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1">
       <c r="A13" s="25" t="s">
@@ -4768,12 +4768,12 @@
       <c r="C13" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="42"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="42"/>
-      <c r="G13" s="42"/>
-      <c r="H13" s="42"/>
-      <c r="I13" s="42"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="47"/>
+      <c r="F13" s="47"/>
+      <c r="G13" s="47"/>
+      <c r="H13" s="47"/>
+      <c r="I13" s="47"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="25" t="s">
@@ -4785,12 +4785,12 @@
       <c r="C14" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="42"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="42"/>
-      <c r="G14" s="42"/>
-      <c r="H14" s="42"/>
-      <c r="I14" s="42"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="47"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="47"/>
+      <c r="H14" s="47"/>
+      <c r="I14" s="47"/>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="26" t="s">
@@ -4802,57 +4802,57 @@
       <c r="C15" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="43"/>
-      <c r="E15" s="43"/>
-      <c r="F15" s="43"/>
-      <c r="G15" s="43"/>
-      <c r="H15" s="43"/>
-      <c r="I15" s="43"/>
+      <c r="D15" s="48"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="48"/>
+      <c r="H15" s="48"/>
+      <c r="I15" s="48"/>
     </row>
     <row r="16" spans="1:9" ht="30" customHeight="1">
       <c r="A16" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="40" t="s">
+      <c r="B16" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="40"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="40"/>
-      <c r="F16" s="40"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="40"/>
+      <c r="C16" s="45"/>
+      <c r="D16" s="45"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="45"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="45"/>
+      <c r="I16" s="45"/>
     </row>
     <row r="17" spans="1:10" ht="64.5" customHeight="1">
       <c r="A17" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="46" t="s">
+      <c r="B17" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="47"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="47"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
+      <c r="C17" s="52"/>
+      <c r="D17" s="52"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="52"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="52"/>
+      <c r="I17" s="52"/>
     </row>
     <row r="18" spans="1:10" ht="30" customHeight="1">
       <c r="A18" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="40" t="s">
+      <c r="B18" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
-      <c r="F18" s="40"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="45"/>
+      <c r="I18" s="45"/>
     </row>
     <row r="19" spans="1:10" s="32" customFormat="1" ht="30">
       <c r="A19" s="3" t="s">
@@ -14417,11 +14417,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -14429,6 +14424,11 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A383:I383 A374:K382 A20:J60 I302:I356 I64:I291 J61:J357 A61:H357 A358:J373">
@@ -14654,12 +14654,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -14708,6 +14702,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -14718,20 +14718,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14746,6 +14732,20 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Update RS,xml and add new test case 'MSWWSP_S03_TC04_AlterToDo_TaskDataNotPresent' for MS-WWSP_R418002
</commit_message>
<xml_diff>
--- a/SharePoint/Docs/MS-WWSP/MS-WWSP_RequirementSpecification.xlsx
+++ b/SharePoint/Docs/MS-WWSP/MS-WWSP_RequirementSpecification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fanff\source\repos\MAPITEST-Interop-TestSuites\SharePoint\Docs\MS-WWSP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F98E75B5-487C-4A69-B4A9-4405F07ABECA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61C543DD-6DF7-464C-9AEE-BAEAAB5E11B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2868,9 +2868,6 @@
     <t>MS-WWSP_R418001</t>
   </si>
   <si>
-    <t>MS-WWSP_R418002</t>
-  </si>
-  <si>
     <t>[In Messages] ClaimReleaseTaskSoapIn specifies the request to claim or release a claim on a workflow task.</t>
   </si>
   <si>
@@ -3139,6 +3136,10 @@
   </si>
   <si>
     <t>[In Appendix B: Product Behavior] Unless otherwise specified, the term "MAY" implies that the product does not follow the prescription.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MS-WWSP_R418002</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3420,6 +3421,21 @@
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3443,21 +3459,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4594,10 +4595,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.375" style="10" customWidth="1"/>
+    <col min="1" max="1" width="20" style="10" customWidth="1"/>
     <col min="2" max="2" width="13" style="3" customWidth="1"/>
     <col min="3" max="3" width="85" style="3" customWidth="1"/>
-    <col min="4" max="4" width="28.625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="6" style="3" customWidth="1"/>
     <col min="5" max="5" width="12.375" style="3" customWidth="1"/>
     <col min="6" max="6" width="12.125" style="3" customWidth="1"/>
     <col min="7" max="7" width="13.375" style="3" customWidth="1"/>
@@ -4641,120 +4642,120 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="48"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="48"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="51" t="s">
+      <c r="B5" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
-      <c r="G5" s="52"/>
-      <c r="H5" s="52"/>
-      <c r="I5" s="52"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="44"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="50"/>
-      <c r="G6" s="50"/>
-      <c r="H6" s="50"/>
-      <c r="I6" s="50"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="42"/>
+      <c r="I6" s="42"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="49" t="s">
+      <c r="B7" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="49"/>
-      <c r="D7" s="49"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49"/>
-      <c r="G7" s="49"/>
-      <c r="H7" s="49"/>
-      <c r="I7" s="49"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="41"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="49" t="s">
+      <c r="B8" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="49"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="49"/>
-      <c r="G8" s="49"/>
-      <c r="H8" s="49"/>
-      <c r="I8" s="49"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
     </row>
     <row r="9" spans="1:9" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="44" t="s">
+      <c r="B9" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="45"/>
-      <c r="D9" s="45"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="45"/>
-      <c r="G9" s="45"/>
-      <c r="H9" s="45"/>
-      <c r="I9" s="45"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="50"/>
+      <c r="I9" s="50"/>
     </row>
     <row r="10" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="44" t="s">
+      <c r="B10" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="45"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="45"/>
-      <c r="G10" s="45"/>
-      <c r="H10" s="45"/>
-      <c r="I10" s="45"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="50"/>
+      <c r="G10" s="50"/>
+      <c r="H10" s="50"/>
+      <c r="I10" s="50"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="45"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="45"/>
+      <c r="I11" s="45"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="24" t="s">
@@ -4766,12 +4767,12 @@
       <c r="C12" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="41"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="41"/>
-      <c r="I12" s="41"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="46"/>
+      <c r="I12" s="46"/>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="25" t="s">
@@ -4783,12 +4784,12 @@
       <c r="C13" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="42"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="42"/>
-      <c r="G13" s="42"/>
-      <c r="H13" s="42"/>
-      <c r="I13" s="42"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="47"/>
+      <c r="F13" s="47"/>
+      <c r="G13" s="47"/>
+      <c r="H13" s="47"/>
+      <c r="I13" s="47"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
@@ -4800,12 +4801,12 @@
       <c r="C14" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="42"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="42"/>
-      <c r="G14" s="42"/>
-      <c r="H14" s="42"/>
-      <c r="I14" s="42"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="47"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="47"/>
+      <c r="H14" s="47"/>
+      <c r="I14" s="47"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="26" t="s">
@@ -4817,57 +4818,57 @@
       <c r="C15" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="43"/>
-      <c r="E15" s="43"/>
-      <c r="F15" s="43"/>
-      <c r="G15" s="43"/>
-      <c r="H15" s="43"/>
-      <c r="I15" s="43"/>
+      <c r="D15" s="48"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="48"/>
+      <c r="H15" s="48"/>
+      <c r="I15" s="48"/>
     </row>
     <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="40" t="s">
+      <c r="B16" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="40"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="40"/>
-      <c r="F16" s="40"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="40"/>
+      <c r="C16" s="45"/>
+      <c r="D16" s="45"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="45"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="45"/>
+      <c r="I16" s="45"/>
     </row>
     <row r="17" spans="1:10" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="46" t="s">
+      <c r="B17" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="47"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="47"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
+      <c r="C17" s="52"/>
+      <c r="D17" s="52"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="52"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="52"/>
+      <c r="I17" s="52"/>
     </row>
     <row r="18" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="40" t="s">
+      <c r="B18" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
-      <c r="F18" s="40"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="45"/>
+      <c r="I18" s="45"/>
     </row>
     <row r="19" spans="1:10" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
@@ -4960,7 +4961,7 @@
         <v>2.1</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="D22" s="21"/>
       <c r="E22" s="21" t="s">
@@ -4986,7 +4987,7 @@
         <v>2.1</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="D23" s="21"/>
       <c r="E23" s="21" t="s">
@@ -5012,7 +5013,7 @@
         <v>2.1</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="D24" s="21"/>
       <c r="E24" s="21" t="s">
@@ -5064,7 +5065,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="D26" s="21"/>
       <c r="E26" s="21" t="s">
@@ -5246,7 +5247,7 @@
         <v>55</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="D33" s="21"/>
       <c r="E33" s="21" t="s">
@@ -5298,7 +5299,7 @@
         <v>55</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="D35" s="21"/>
       <c r="E35" s="21" t="s">
@@ -5324,7 +5325,7 @@
         <v>55</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="D36" s="21"/>
       <c r="E36" s="21" t="s">
@@ -6706,7 +6707,7 @@
         <v>32</v>
       </c>
       <c r="C89" s="19" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="D89" s="21"/>
       <c r="E89" s="21" t="s">
@@ -7170,7 +7171,7 @@
     </row>
     <row r="107" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A107" s="21" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="B107" s="22" t="s">
         <v>210</v>
@@ -7328,13 +7329,13 @@
     </row>
     <row r="113" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A113" s="21" t="s">
-        <v>788</v>
+        <v>831</v>
       </c>
       <c r="B113" s="22" t="s">
         <v>210</v>
       </c>
       <c r="C113" s="19" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="D113" s="31"/>
       <c r="E113" s="21" t="s">
@@ -7347,7 +7348,7 @@
         <v>15</v>
       </c>
       <c r="H113" s="31" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I113" s="38"/>
       <c r="J113" s="19"/>
@@ -7360,7 +7361,7 @@
         <v>229</v>
       </c>
       <c r="C114" s="19" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="D114" s="21"/>
       <c r="E114" s="21" t="s">
@@ -7542,7 +7543,7 @@
         <v>33</v>
       </c>
       <c r="C121" s="19" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="D121" s="21"/>
       <c r="E121" s="21" t="s">
@@ -7646,7 +7647,7 @@
         <v>247</v>
       </c>
       <c r="C125" s="19" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="D125" s="21"/>
       <c r="E125" s="21" t="s">
@@ -7672,7 +7673,7 @@
         <v>247</v>
       </c>
       <c r="C126" s="19" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="D126" s="21"/>
       <c r="E126" s="21" t="s">
@@ -7854,7 +7855,7 @@
         <v>263</v>
       </c>
       <c r="C133" s="19" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="D133" s="21"/>
       <c r="E133" s="21" t="s">
@@ -7880,7 +7881,7 @@
         <v>263</v>
       </c>
       <c r="C134" s="19" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="D134" s="21"/>
       <c r="E134" s="21" t="s">
@@ -7932,7 +7933,7 @@
         <v>267</v>
       </c>
       <c r="C136" s="19" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="D136" s="21"/>
       <c r="E136" s="21" t="s">
@@ -8326,7 +8327,7 @@
         <v>289</v>
       </c>
       <c r="C151" s="19" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="D151" s="21"/>
       <c r="E151" s="21" t="s">
@@ -8924,7 +8925,7 @@
         <v>347</v>
       </c>
       <c r="C174" s="19" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="D174" s="21"/>
       <c r="E174" s="21" t="s">
@@ -9444,7 +9445,7 @@
         <v>391</v>
       </c>
       <c r="C194" s="19" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="D194" s="21"/>
       <c r="E194" s="21" t="s">
@@ -9990,7 +9991,7 @@
         <v>437</v>
       </c>
       <c r="C215" s="19" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="D215" s="21"/>
       <c r="E215" s="21" t="s">
@@ -11628,7 +11629,7 @@
         <v>437</v>
       </c>
       <c r="C278" s="19" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="D278" s="21"/>
       <c r="E278" s="21" t="s">
@@ -11682,7 +11683,7 @@
         <v>437</v>
       </c>
       <c r="C280" s="19" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="D280" s="21"/>
       <c r="E280" s="21" t="s">
@@ -11730,13 +11731,13 @@
     </row>
     <row r="282" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A282" s="21" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="B282" s="22" t="s">
         <v>437</v>
       </c>
       <c r="C282" s="39" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="D282" s="31"/>
       <c r="E282" s="21" t="s">
@@ -12754,7 +12755,7 @@
         <v>618</v>
       </c>
       <c r="C321" s="19" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="D321" s="21"/>
       <c r="E321" s="21" t="s">
@@ -12858,7 +12859,7 @@
         <v>635</v>
       </c>
       <c r="C325" s="19" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="D325" s="21"/>
       <c r="E325" s="21" t="s">
@@ -13034,13 +13035,13 @@
     </row>
     <row r="332" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A332" s="21" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B332" s="22" t="s">
         <v>645</v>
       </c>
       <c r="C332" s="39" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="D332" s="31"/>
       <c r="E332" s="21" t="s">
@@ -13534,7 +13535,7 @@
         <v>674</v>
       </c>
       <c r="C351" s="19" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="D351" s="21"/>
       <c r="E351" s="21" t="s">
@@ -13554,13 +13555,13 @@
     </row>
     <row r="352" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A352" s="21" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="B352" s="22" t="s">
         <v>674</v>
       </c>
       <c r="C352" s="39" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="D352" s="31"/>
       <c r="E352" s="31" t="s">
@@ -13750,7 +13751,7 @@
         <v>7</v>
       </c>
       <c r="C359" s="19" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="D359" s="21"/>
       <c r="E359" s="21" t="s">
@@ -13776,7 +13777,7 @@
         <v>7</v>
       </c>
       <c r="C360" s="19" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="D360" s="21"/>
       <c r="E360" s="21" t="s">
@@ -13802,7 +13803,7 @@
         <v>7</v>
       </c>
       <c r="C361" s="19" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="D361" s="21"/>
       <c r="E361" s="21" t="s">
@@ -13828,7 +13829,7 @@
         <v>7</v>
       </c>
       <c r="C362" s="19" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="D362" s="21"/>
       <c r="E362" s="21" t="s">
@@ -13854,7 +13855,7 @@
         <v>7</v>
       </c>
       <c r="C363" s="19" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="D363" s="21"/>
       <c r="E363" s="21" t="s">
@@ -13880,7 +13881,7 @@
         <v>7</v>
       </c>
       <c r="C364" s="19" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="D364" s="21"/>
       <c r="E364" s="21" t="s">
@@ -13906,7 +13907,7 @@
         <v>7</v>
       </c>
       <c r="C365" s="19" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="D365" s="21"/>
       <c r="E365" s="21" t="s">
@@ -13958,7 +13959,7 @@
         <v>7</v>
       </c>
       <c r="C367" s="19" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="D367" s="21"/>
       <c r="E367" s="21" t="s">
@@ -13984,7 +13985,7 @@
         <v>7</v>
       </c>
       <c r="C368" s="19" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="D368" s="21" t="s">
         <v>767</v>
@@ -14042,7 +14043,7 @@
         <v>7</v>
       </c>
       <c r="C370" s="19" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="D370" s="21" t="s">
         <v>768</v>
@@ -14102,7 +14103,7 @@
         <v>7</v>
       </c>
       <c r="C372" s="19" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="D372" s="21" t="s">
         <v>769</v>
@@ -14432,11 +14433,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -14444,6 +14440,11 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A383:I383 A374:K382 A20:J60 I302:I356 I64:I291 J61:J357 A61:H357 A358:J373">
@@ -14669,9 +14670,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -14724,24 +14728,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -14762,9 +14757,15 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>